<commit_message>
wu yu guo shi zhu
</commit_message>
<xml_diff>
--- a/记录.xlsx
+++ b/记录.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="436">
   <si>
     <t>前程无忧</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1706,6 +1706,10 @@
   </si>
   <si>
     <t>http://www.yingjiesheng.com/job-001-435-491.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>abc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2381,7 +2385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
@@ -4593,6 +4597,11 @@
       </c>
       <c r="E134" s="3" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="3" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>